<commit_message>
Update $ADSK, update Tech overview
</commit_message>
<xml_diff>
--- a/$ESTC.xlsx
+++ b/$ESTC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE04C68-5AF1-4DEA-9709-1DACDBCA9F4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DFF5D7-19E1-47E3-BB08-4F52DA3674B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C17CCCFF-BC06-47D8-B432-71950F7FA339}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C17CCCFF-BC06-47D8-B432-71950F7FA339}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="101">
   <si>
     <t>$ESTC</t>
   </si>
@@ -326,6 +326,9 @@
   </si>
   <si>
     <t>Q425</t>
+  </si>
+  <si>
+    <t>Mountain View, CA</t>
   </si>
 </sst>
 </file>
@@ -511,7 +514,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -569,6 +572,9 @@
     <xf numFmtId="15" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -588,6 +594,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -913,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{691FEFE0-031E-449B-9B3E-DEA7EAB8B130}">
   <dimension ref="B2:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -938,11 +950,11 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
@@ -958,10 +970,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="3">
-        <f>+'Financial Model'!K24</f>
-        <v>102.284435</v>
-      </c>
-      <c r="D7" s="5"/>
+        <f>+'Financial Model'!L24</f>
+        <v>103.23874000000001</v>
+      </c>
+      <c r="D7" s="27" t="str">
+        <f>+$C$29</f>
+        <v>Q225</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
@@ -969,7 +984,7 @@
       </c>
       <c r="C8" s="3">
         <f>C6*C7</f>
-        <v>9527.7951202500008</v>
+        <v>9616.6886310000009</v>
       </c>
       <c r="D8" s="5"/>
     </row>
@@ -981,7 +996,10 @@
         <f>+'Financial Model'!K73</f>
         <v>1147.33</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="27" t="str">
+        <f t="shared" ref="D9:D11" si="0">+$C$29</f>
+        <v>Q225</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
@@ -991,7 +1009,10 @@
         <f>+'Financial Model'!K74</f>
         <v>568.88699999999994</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>Q225</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
@@ -1001,7 +1022,10 @@
         <f>C9-C10</f>
         <v>578.44299999999998</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>Q225</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
@@ -1009,142 +1033,151 @@
       </c>
       <c r="C12" s="7">
         <f>C8-C11</f>
-        <v>8949.3521202500015</v>
+        <v>9038.2456310000016</v>
       </c>
       <c r="D12" s="8"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="11"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="29"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="11"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="11"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="13"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="34"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="32"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="28"/>
+      <c r="C23" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="29"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="28"/>
+      <c r="C24" s="35">
+        <v>2012</v>
+      </c>
+      <c r="D24" s="36"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="28"/>
+      <c r="C25" s="35">
+        <v>2018</v>
+      </c>
+      <c r="D25" s="36"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="14"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="29"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="29"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="14"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="29"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="14" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D29" s="26">
-        <v>45524</v>
+        <f>+'Financial Model'!L3</f>
+        <v>45617</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="34"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="32"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="34">
+      <c r="C34" s="37">
         <f>+C6/'Financial Model'!K71</f>
         <v>12.550196094773931</v>
       </c>
-      <c r="D34" s="35"/>
+      <c r="D34" s="38"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="29"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="27"/>
-      <c r="D36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="29"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="14"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="29"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="28"/>
+      <c r="C38" s="28">
+        <v>64</v>
+      </c>
+      <c r="D38" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -1178,7 +1211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8FF81E-C7BC-429A-AF70-7B66A6FE5D82}">
   <dimension ref="A1:U88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -1367,7 +1400,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="20">
-        <f t="shared" ref="C6:J6" si="0">+C4+C5</f>
+        <f t="shared" ref="C6:I6" si="0">+C4+C5</f>
         <v>0</v>
       </c>
       <c r="D6" s="20">
@@ -1494,7 +1527,7 @@
         <v>37</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" ref="C9:J9" si="1">+C7+C8</f>
+        <f t="shared" ref="C9:I9" si="1">+C7+C8</f>
         <v>0</v>
       </c>
       <c r="D9" s="3">
@@ -1543,7 +1576,7 @@
         <v>38</v>
       </c>
       <c r="C10" s="20">
-        <f t="shared" ref="C10:J10" si="2">+C6-C9</f>
+        <f t="shared" ref="C10:I10" si="2">+C6-C9</f>
         <v>0</v>
       </c>
       <c r="D10" s="20">
@@ -1592,7 +1625,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" ref="C11:J11" si="3">+C4-C7</f>
+        <f t="shared" ref="C11:I11" si="3">+C4-C7</f>
         <v>0</v>
       </c>
       <c r="D11" s="3">
@@ -1620,15 +1653,15 @@
         <v>243.65600000000001</v>
       </c>
       <c r="J11" s="3">
-        <f>+J4-J7</f>
+        <f t="shared" ref="J11:L12" si="4">+J4-J7</f>
         <v>245.93699999999998</v>
       </c>
       <c r="K11" s="3">
-        <f>+K4-K7</f>
+        <f t="shared" si="4"/>
         <v>255.42700000000002</v>
       </c>
       <c r="L11" s="3">
-        <f>+L4-L7</f>
+        <f t="shared" si="4"/>
         <v>270.86599999999999</v>
       </c>
       <c r="T11" s="3">
@@ -1641,15 +1674,15 @@
         <v>61</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" ref="C12:J12" si="4">+C5-C8</f>
+        <f t="shared" ref="C12:I12" si="5">+C5-C8</f>
         <v>0</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.10900000000000176</v>
       </c>
       <c r="F12" s="3">
@@ -1657,27 +1690,27 @@
         <v>4.6430000000000007</v>
       </c>
       <c r="G12" s="3">
+        <f t="shared" si="5"/>
+        <v>3.2950000000000017</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="5"/>
+        <v>2.7759999999999998</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="5"/>
+        <v>-0.34100000000000108</v>
+      </c>
+      <c r="J12" s="3">
         <f t="shared" si="4"/>
-        <v>3.2950000000000017</v>
-      </c>
-      <c r="H12" s="3">
+        <v>1.1909999999999989</v>
+      </c>
+      <c r="K12" s="3">
         <f t="shared" si="4"/>
-        <v>2.7759999999999998</v>
-      </c>
-      <c r="I12" s="3">
+        <v>0.23600000000000065</v>
+      </c>
+      <c r="L12" s="3">
         <f t="shared" si="4"/>
-        <v>-0.34100000000000108</v>
-      </c>
-      <c r="J12" s="3">
-        <f>+J5-J8</f>
-        <v>1.1909999999999989</v>
-      </c>
-      <c r="K12" s="3">
-        <f>+K5-K8</f>
-        <v>0.23600000000000065</v>
-      </c>
-      <c r="L12" s="3">
-        <f>+L5-L8</f>
         <v>1.3159999999999989</v>
       </c>
       <c r="T12" s="3">
@@ -1822,15 +1855,15 @@
         <v>43</v>
       </c>
       <c r="C17" s="20">
-        <f t="shared" ref="C17:J17" si="5">+C10-SUM(C13:C16)</f>
+        <f t="shared" ref="C17:I17" si="6">+C10-SUM(C13:C16)</f>
         <v>0</v>
       </c>
       <c r="D17" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E17" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-69.347000000000008</v>
       </c>
       <c r="F17" s="20">
@@ -1838,15 +1871,15 @@
         <v>-40.155999999999977</v>
       </c>
       <c r="G17" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-36.246999999999957</v>
       </c>
       <c r="H17" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-21.539000000000016</v>
       </c>
       <c r="I17" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-26.403999999999996</v>
       </c>
       <c r="J17" s="20">
@@ -1937,15 +1970,15 @@
         <v>45</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" ref="C20:J20" si="6">+C17-C18+C19</f>
+        <f t="shared" ref="C20:I20" si="7">+C17-C18+C19</f>
         <v>0</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-70.152000000000015</v>
       </c>
       <c r="F20" s="3">
@@ -1953,15 +1986,15 @@
         <v>-39.759999999999977</v>
       </c>
       <c r="G20" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-35.252999999999957</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-19.649000000000015</v>
       </c>
       <c r="I20" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-24.204000000000001</v>
       </c>
       <c r="J20" s="3">
@@ -2019,15 +2052,15 @@
         <v>47</v>
       </c>
       <c r="C22" s="20">
-        <f t="shared" ref="C22:J22" si="7">+C20-C21</f>
+        <f t="shared" ref="C22:I22" si="8">+C20-C21</f>
         <v>0</v>
       </c>
       <c r="D22" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E22" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-72.574000000000012</v>
       </c>
       <c r="F22" s="20">
@@ -2035,15 +2068,15 @@
         <v>-46.73099999999998</v>
       </c>
       <c r="G22" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-48.50799999999996</v>
       </c>
       <c r="H22" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-24.796000000000014</v>
       </c>
       <c r="I22" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>176.124</v>
       </c>
       <c r="J22" s="20">
@@ -2068,35 +2101,35 @@
         <v>48</v>
       </c>
       <c r="E23" s="21">
-        <f>+E22/E24</f>
+        <f t="shared" ref="E23:L23" si="9">+E22/E24</f>
         <v>-0.75556970298127513</v>
       </c>
       <c r="F23" s="21">
-        <f>+F22/F24</f>
+        <f t="shared" si="9"/>
         <v>-0.48187196353302347</v>
       </c>
       <c r="G23" s="21">
-        <f>+G22/G24</f>
+        <f t="shared" si="9"/>
         <v>-0.49527246463875757</v>
       </c>
       <c r="H23" s="21">
-        <f>+H22/H24</f>
+        <f t="shared" si="9"/>
         <v>-0.25027908348477923</v>
       </c>
       <c r="I23" s="21">
-        <f>+I22/I24</f>
+        <f t="shared" si="9"/>
         <v>1.7562841349907246</v>
       </c>
       <c r="J23" s="21">
-        <f>+J22/J24</f>
+        <f t="shared" si="9"/>
         <v>-0.40563042266068267</v>
       </c>
       <c r="K23" s="21">
-        <f>+K22/K24</f>
+        <f t="shared" si="9"/>
         <v>-0.48127557237814295</v>
       </c>
       <c r="L23" s="21">
-        <f>+L22/L24</f>
+        <f t="shared" si="9"/>
         <v>-0.24651598808741745</v>
       </c>
       <c r="T23" s="21">
@@ -2142,23 +2175,23 @@
         <v>55</v>
       </c>
       <c r="E26" s="22">
-        <f>+E11/E4</f>
+        <f t="shared" ref="E26:G27" si="10">+E11/E4</f>
         <v>0.78034763490119818</v>
       </c>
       <c r="F26" s="22">
-        <f>+F11/F4</f>
+        <f t="shared" si="10"/>
         <v>0.78718120910184131</v>
       </c>
       <c r="G26" s="22">
-        <f>+G11/G4</f>
+        <f t="shared" si="10"/>
         <v>0.78809755519950275</v>
       </c>
       <c r="H26" s="22">
-        <f t="shared" ref="H26:I27" si="8">+H11/H4</f>
+        <f t="shared" ref="H26:I27" si="11">+H11/H4</f>
         <v>0.79149449334996846</v>
       </c>
       <c r="I26" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.79203723929890257</v>
       </c>
       <c r="J26" s="22">
@@ -2170,11 +2203,11 @@
         <v>0.78890522401428165</v>
       </c>
       <c r="L26" s="22">
-        <f t="shared" ref="L26:L27" si="9">+L11/L4</f>
+        <f t="shared" ref="L26:L27" si="12">+L11/L4</f>
         <v>0.79477827626779962</v>
       </c>
       <c r="T26" s="22">
-        <f t="shared" ref="T26:T27" si="10">+T11/T4</f>
+        <f t="shared" ref="T26:T27" si="13">+T11/T4</f>
         <v>0.79068184251992601</v>
       </c>
     </row>
@@ -2183,23 +2216,23 @@
         <v>56</v>
       </c>
       <c r="E27" s="22">
-        <f>+E12/E5</f>
+        <f t="shared" si="10"/>
         <v>-5.75106843243823E-3</v>
       </c>
       <c r="F27" s="22">
-        <f>+F12/F5</f>
+        <f t="shared" si="10"/>
         <v>0.19494478733677628</v>
       </c>
       <c r="G27" s="22">
-        <f>+G12/G5</f>
+        <f t="shared" si="10"/>
         <v>0.14017697609121083</v>
       </c>
       <c r="H27" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.12138703047793956</v>
       </c>
       <c r="I27" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-1.677736777367779E-2</v>
       </c>
       <c r="J27" s="22">
@@ -2211,11 +2244,11 @@
         <v>9.9805463926245733E-3</v>
       </c>
       <c r="L27" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>5.3596155412560034E-2</v>
       </c>
       <c r="T27" s="22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>7.6293887449705194E-2</v>
       </c>
     </row>
@@ -2236,11 +2269,11 @@
         <v>0.73625120424302049</v>
       </c>
       <c r="H29" s="22">
-        <f t="shared" ref="H29:I29" si="11">+H10/H6</f>
+        <f t="shared" ref="H29:I29" si="14">+H10/H6</f>
         <v>0.7421574182581484</v>
       </c>
       <c r="I29" s="22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.74191128715044963</v>
       </c>
       <c r="J29" s="22">
@@ -2252,11 +2285,11 @@
         <v>0.73589027689827868</v>
       </c>
       <c r="L29" s="22">
-        <f t="shared" ref="L29" si="12">+L10/L6</f>
+        <f t="shared" ref="L29" si="15">+L10/L6</f>
         <v>0.74496730630800778</v>
       </c>
       <c r="T29" s="22">
-        <f t="shared" ref="T29" si="13">+T10/T6</f>
+        <f t="shared" ref="T29" si="16">+T10/T6</f>
         <v>0.73954586091448027</v>
       </c>
     </row>
@@ -2277,11 +2310,11 @@
         <v>-0.12339278237158413</v>
       </c>
       <c r="H30" s="22">
-        <f t="shared" ref="H30:I30" si="14">+H17/H6</f>
+        <f t="shared" ref="H30:I30" si="17">+H17/H6</f>
         <v>-6.9343747182980753E-2</v>
       </c>
       <c r="I30" s="22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-8.0510554737358853E-2</v>
       </c>
       <c r="J30" s="22">
@@ -2293,11 +2326,11 @@
         <v>-9.7397962120775908E-2</v>
       </c>
       <c r="L30" s="22">
-        <f t="shared" ref="L30" si="15">+L17/L6</f>
+        <f t="shared" ref="L30" si="18">+L17/L6</f>
         <v>-1.2114046107822093E-2</v>
       </c>
       <c r="T30" s="22">
-        <f t="shared" ref="T30" si="16">+T17/T6</f>
+        <f t="shared" ref="T30" si="19">+T17/T6</f>
         <v>-0.10250126053304555</v>
       </c>
     </row>
@@ -2318,11 +2351,11 @@
         <v>-0.16513193056751746</v>
       </c>
       <c r="H31" s="22">
-        <f t="shared" ref="H31:I31" si="17">+H22/H6</f>
+        <f t="shared" ref="H31:I31" si="20">+H22/H6</f>
         <v>-7.9829497894479337E-2</v>
       </c>
       <c r="I31" s="22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>0.53703381845790754</v>
       </c>
       <c r="J31" s="22">
@@ -2334,11 +2367,11 @@
         <v>-0.141693051637787</v>
       </c>
       <c r="L31" s="22">
-        <f t="shared" ref="L31" si="18">+L22/L6</f>
+        <f t="shared" ref="L31" si="21">+L22/L6</f>
         <v>-6.9657133629478757E-2</v>
       </c>
       <c r="T31" s="22">
-        <f t="shared" ref="T31" si="19">+T22/T6</f>
+        <f t="shared" ref="T31" si="22">+T22/T6</f>
         <v>4.8701157796643607E-2</v>
       </c>
     </row>
@@ -2359,11 +2392,11 @@
         <v>-0.37599636910333922</v>
       </c>
       <c r="H32" s="22">
-        <f t="shared" ref="H32:I32" si="20">+H21/H20</f>
+        <f t="shared" ref="H32:I32" si="23">+H21/H20</f>
         <v>-0.26194717288411606</v>
       </c>
       <c r="I32" s="22">
-        <f t="shared" si="20"/>
+        <f t="shared" si="23"/>
         <v>8.2766484878532474</v>
       </c>
       <c r="J32" s="22">
@@ -2375,11 +2408,11 @@
         <v>-0.68840032926327432</v>
       </c>
       <c r="L32" s="22">
-        <f t="shared" ref="L32" si="21">+L21/L20</f>
+        <f t="shared" ref="L32" si="24">+L21/L20</f>
         <v>-13.281705948372707</v>
       </c>
       <c r="T32" s="22">
-        <f t="shared" ref="T32" si="22">+T21/T20</f>
+        <f t="shared" ref="T32" si="25">+T21/T20</f>
         <v>1.5027860145328966</v>
       </c>
     </row>
@@ -2409,11 +2442,11 @@
         <v>97</v>
       </c>
       <c r="H35" s="22">
-        <f t="shared" ref="H35:I35" si="23">+H6/G6-1</f>
+        <f t="shared" ref="H35:I35" si="26">+H6/G6-1</f>
         <v>5.7391754296977071E-2</v>
       </c>
       <c r="I35" s="22">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>5.5841371228413594E-2</v>
       </c>
       <c r="L35" s="22">

</xml_diff>